<commit_message>
Completed test_Add_employee test case
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_Testdata.xlsx
+++ b/testData/OrangeHRM_Testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\OrangeHRM\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Automation_Work\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D250DB6A-259E-44F9-934F-3E8D97667334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9833D718-38ED-4B37-9599-7A18487DD795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
   </bookViews>
@@ -76,16 +76,16 @@
     <t>A</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>Ajay</t>
-  </si>
-  <si>
-    <t>Ajay@20</t>
-  </si>
-  <si>
-    <t>Ajay_kumar</t>
+    <t>Angra</t>
+  </si>
+  <si>
+    <t>Nishchay</t>
+  </si>
+  <si>
+    <t>Nishchay_Angra</t>
+  </si>
+  <si>
+    <t>Nishchay@20</t>
   </si>
 </sst>
 </file>
@@ -545,11 +545,12 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
@@ -592,19 +593,18 @@
         <v>1824</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{50C0D8A5-1226-423F-95D8-1DBA26EDD766}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{EFAEA3F0-58D3-481F-A9C4-F1469F6715A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
In Progress test_Employee_details test case
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_Testdata.xlsx
+++ b/testData/OrangeHRM_Testdata.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Automation_Work\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9833D718-38ED-4B37-9599-7A18487DD795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB0A92E-7639-4D78-A074-FA6F89044129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="PIM_Add_Employee" sheetId="2" r:id="rId2"/>
+    <sheet name="Employee_Details" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>url</t>
   </si>
@@ -76,23 +77,86 @@
     <t>A</t>
   </si>
   <si>
-    <t>Angra</t>
-  </si>
-  <si>
-    <t>Nishchay</t>
-  </si>
-  <si>
-    <t>Nishchay_Angra</t>
-  </si>
-  <si>
-    <t>Nishchay@20</t>
+    <t>otherid</t>
+  </si>
+  <si>
+    <t>drivinglicence</t>
+  </si>
+  <si>
+    <t>licexpdate</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>DL29AC2389</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>licexpmonth</t>
+  </si>
+  <si>
+    <t>licexpyear</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>Arora</t>
+  </si>
+  <si>
+    <t>maritalstatus</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>dobmonth</t>
+  </si>
+  <si>
+    <t>dobyear</t>
+  </si>
+  <si>
+    <t>dobdate</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Sweta</t>
+  </si>
+  <si>
+    <t>Sweta@20</t>
+  </si>
+  <si>
+    <t>bloodtype</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>testfield</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Sweta@Arora_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +182,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -180,6 +251,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -545,7 +621,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,31 +657,142 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
-        <v>1824</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>2965</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{50C0D8A5-1226-423F-95D8-1DBA26EDD766}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{DD30683B-4C77-4C64-84A0-5CE441B39DD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9363D7-1F1E-4512-871E-F77607C61FFA}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2023</v>
+      </c>
+      <c r="F2" s="2">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1995</v>
+      </c>
+      <c r="J2" s="2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Add Personal Details test case
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_Testdata.xlsx
+++ b/testData/OrangeHRM_Testdata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Automation_Work\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB0A92E-7639-4D78-A074-FA6F89044129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB23C1F7-A2A0-4653-98AF-EC0787A0128E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="PIM_Add_Employee" sheetId="2" r:id="rId2"/>
-    <sheet name="Employee_Details" sheetId="3" r:id="rId3"/>
+    <sheet name="Employee_Personal_Details" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>url</t>
   </si>
@@ -104,9 +104,6 @@
     <t>August</t>
   </si>
   <si>
-    <t>Arora</t>
-  </si>
-  <si>
     <t>maritalstatus</t>
   </si>
   <si>
@@ -131,12 +128,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Sweta</t>
-  </si>
-  <si>
-    <t>Sweta@20</t>
-  </si>
-  <si>
     <t>bloodtype</t>
   </si>
   <si>
@@ -149,7 +140,22 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Sweta@Arora_10</t>
+    <t>Geeta</t>
+  </si>
+  <si>
+    <t>Angra</t>
+  </si>
+  <si>
+    <t>Geeta@20</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Personal Details have been added.</t>
+  </si>
+  <si>
+    <t>Geeta@Angra_30</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -236,6 +242,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -252,10 +267,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -657,25 +672,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2">
         <v>2965</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -689,10 +704,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9363D7-1F1E-4512-871E-F77607C61FFA}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,9 +722,10 @@
     <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -729,28 +745,31 @@
         <v>18</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>38</v>
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>12</v>
       </c>
@@ -770,10 +789,10 @@
         <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2">
         <v>1995</v>
@@ -782,13 +801,16 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Add Contact Details test case
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_Testdata.xlsx
+++ b/testData/OrangeHRM_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Automation_Work\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB23C1F7-A2A0-4653-98AF-EC0787A0128E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91347766-7B64-422A-8359-302F5EE3DBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="PIM_Add_Employee" sheetId="2" r:id="rId2"/>
     <sheet name="Employee_Personal_Details" sheetId="3" r:id="rId3"/>
+    <sheet name="Employee_Contact_Details" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>url</t>
   </si>
@@ -140,22 +141,79 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Geeta</t>
-  </si>
-  <si>
-    <t>Angra</t>
-  </si>
-  <si>
-    <t>Geeta@20</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
     <t>Personal Details have been added.</t>
   </si>
   <si>
-    <t>Geeta@Angra_30</t>
+    <t>street1</t>
+  </si>
+  <si>
+    <t>street2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>telephonehome</t>
+  </si>
+  <si>
+    <t>telephonemobile</t>
+  </si>
+  <si>
+    <t>telephonework</t>
+  </si>
+  <si>
+    <t>workemail</t>
+  </si>
+  <si>
+    <t>otheremail</t>
+  </si>
+  <si>
+    <t>C-119,NDMC Society</t>
+  </si>
+  <si>
+    <t>H-Block,Vikas Puri</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>This is the test automation Framework</t>
+  </si>
+  <si>
+    <t>nishchay1@gmail.com</t>
+  </si>
+  <si>
+    <t>angra1@gmail.com</t>
+  </si>
+  <si>
+    <t>Vishal</t>
+  </si>
+  <si>
+    <t>Arora</t>
+  </si>
+  <si>
+    <t>Vishal_Arora</t>
+  </si>
+  <si>
+    <t>Vishal@20</t>
   </si>
 </sst>
 </file>
@@ -256,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -270,7 +328,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,7 +698,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,31 +734,32 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2">
-        <v>2965</v>
+        <v>6321</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{50C0D8A5-1226-423F-95D8-1DBA26EDD766}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{DD30683B-4C77-4C64-84A0-5CE441B39DD5}"/>
+    <hyperlink ref="E2" r:id="rId2" display="Geeta@Angra" xr:uid="{DD30683B-4C77-4C64-84A0-5CE441B39DD5}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{C4B77C74-F810-4E1C-AB8A-1F74AFC6841D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -707,7 +770,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +829,7 @@
         <v>35</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -810,11 +873,120 @@
         <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A595981-FC99-4278-B0DC-0B43D98197D1}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2">
+        <v>110018</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2345465577</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3454656533</v>
+      </c>
+      <c r="I2" s="2">
+        <v>34534654654</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{86A26AA3-4120-4524-9FBC-52F2A5291109}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{3BA578BE-9B57-4B3C-A5EB-CEE2E72611E2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Add Emergency Contacts test case
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_Testdata.xlsx
+++ b/testData/OrangeHRM_Testdata.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Automation_Work\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91347766-7B64-422A-8359-302F5EE3DBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B78BA7A-43F6-48CC-9588-0F4390EEB64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="PIM_Add_Employee" sheetId="2" r:id="rId2"/>
     <sheet name="Employee_Personal_Details" sheetId="3" r:id="rId3"/>
     <sheet name="Employee_Contact_Details" sheetId="4" r:id="rId4"/>
+    <sheet name="Emergency_Contacts" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>url</t>
   </si>
@@ -198,22 +199,52 @@
     <t>This is the test automation Framework</t>
   </si>
   <si>
-    <t>nishchay1@gmail.com</t>
-  </si>
-  <si>
-    <t>angra1@gmail.com</t>
-  </si>
-  <si>
-    <t>Vishal</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>Vishal_Arora</t>
-  </si>
-  <si>
-    <t>Vishal@20</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>hometelephone</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>worktelephone</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>He is the father of the Employee.</t>
+  </si>
+  <si>
+    <t>changedcomment</t>
+  </si>
+  <si>
+    <t>He is the gaurdian of the Employee.</t>
+  </si>
+  <si>
+    <t>Druma</t>
+  </si>
+  <si>
+    <t>Vyas</t>
+  </si>
+  <si>
+    <t>Druma@20</t>
+  </si>
+  <si>
+    <t>Druma@gmail.com</t>
+  </si>
+  <si>
+    <t>Vyas@gmail.com</t>
+  </si>
+  <si>
+    <t>DrumaVyas</t>
   </si>
 </sst>
 </file>
@@ -314,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -333,6 +364,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,7 +730,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,32 +766,31 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D2" s="2">
-        <v>6321</v>
+        <v>2002</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{50C0D8A5-1226-423F-95D8-1DBA26EDD766}"/>
     <hyperlink ref="E2" r:id="rId2" display="Geeta@Angra" xr:uid="{DD30683B-4C77-4C64-84A0-5CE441B39DD5}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{C4B77C74-F810-4E1C-AB8A-1F74AFC6841D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -973,10 +1004,10 @@
         <v>34534654654</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>55</v>
@@ -989,4 +1020,74 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939CFAEB-0D2F-4EFD-BB3B-809C383F69FE}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2">
+        <v>98346712</v>
+      </c>
+      <c r="D2" s="2">
+        <v>9023847309</v>
+      </c>
+      <c r="E2" s="2">
+        <v>6719326453</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Add Immigration test case
</commit_message>
<xml_diff>
--- a/testData/OrangeHRM_Testdata.xlsx
+++ b/testData/OrangeHRM_Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Automation_Work\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B78BA7A-43F6-48CC-9588-0F4390EEB64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECE7B3A-D6AA-4BE9-972A-7D2B01EF8A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7413260C-89C3-4F84-BDB9-FE80594C2973}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Employee_Personal_Details" sheetId="3" r:id="rId3"/>
     <sheet name="Employee_Contact_Details" sheetId="4" r:id="rId4"/>
     <sheet name="Emergency_Contacts" sheetId="5" r:id="rId5"/>
+    <sheet name="Dependents" sheetId="6" r:id="rId6"/>
+    <sheet name="Immigration" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="96">
   <si>
     <t>url</t>
   </si>
@@ -127,9 +129,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>bloodtype</t>
   </si>
   <si>
@@ -229,22 +228,97 @@
     <t>He is the gaurdian of the Employee.</t>
   </si>
   <si>
-    <t>Druma</t>
-  </si>
-  <si>
-    <t>Vyas</t>
-  </si>
-  <si>
-    <t>Druma@20</t>
-  </si>
-  <si>
-    <t>Druma@gmail.com</t>
-  </si>
-  <si>
-    <t>Vyas@gmail.com</t>
-  </si>
-  <si>
-    <t>DrumaVyas</t>
+    <t>dependentsname</t>
+  </si>
+  <si>
+    <t>Mayank</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>He is the child of the Employee.</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>issuedby</t>
+  </si>
+  <si>
+    <t>issuedmonth</t>
+  </si>
+  <si>
+    <t>issuedyear</t>
+  </si>
+  <si>
+    <t>issueddate</t>
+  </si>
+  <si>
+    <t>expirymonth</t>
+  </si>
+  <si>
+    <t>expiryyear</t>
+  </si>
+  <si>
+    <t>expirydate</t>
+  </si>
+  <si>
+    <t>eligiblestatus</t>
+  </si>
+  <si>
+    <t>reviewmonth</t>
+  </si>
+  <si>
+    <t>reviewyear</t>
+  </si>
+  <si>
+    <t>reviewdate</t>
+  </si>
+  <si>
+    <t>immigrationcomments</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Employee is eligble for immigration</t>
+  </si>
+  <si>
+    <t>This is the Proof of Immigration</t>
+  </si>
+  <si>
+    <t>Jain</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Jain@gmail.com</t>
+  </si>
+  <si>
+    <t>Rohan@gmail.com</t>
+  </si>
+  <si>
+    <t>Sunil_Jain</t>
+  </si>
+  <si>
+    <t>Sunil@20</t>
   </si>
 </sst>
 </file>
@@ -345,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -364,7 +438,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -730,7 +803,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,25 +839,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="D2" s="2">
-        <v>2002</v>
+        <v>9456</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +874,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,13 +927,13 @@
         <v>31</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -895,16 +968,16 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -939,60 +1012,60 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="L1" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E2" s="2">
         <v>110018</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="2">
         <v>2345465577</v>
@@ -1004,13 +1077,13 @@
         <v>34534654654</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1027,7 +1100,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,33 +1116,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>64</v>
+        <v>36</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="2">
         <v>98346712</v>
@@ -1081,13 +1154,203 @@
         <v>6719326453</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0104A7DE-413B-4EE5-A61C-DCF46DDBE141}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2002</v>
+      </c>
+      <c r="E2" s="2">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD8D903-B80A-4785-B86C-C89CF65874FF}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9812345670</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2035</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2023</v>
+      </c>
+      <c r="M2" s="2">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>